<commit_message>
redo auth to work with xlsx files, and ui test
</commit_message>
<xml_diff>
--- a/data/done.xlsx
+++ b/data/done.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="9527" windowHeight="7835" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="19200" windowHeight="6950" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -38,13 +38,6 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
       <charset val="134"/>
       <b val="1"/>
       <color theme="3"/>
@@ -54,17 +47,16 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <color rgb="FF0000FF"/>
       <sz val="11"/>
       <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -100,6 +92,21 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <charset val="134"/>
       <b val="1"/>
       <color theme="3"/>
@@ -125,7 +132,14 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF006100"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -133,21 +147,7 @@
       <name val="Calibri"/>
       <charset val="0"/>
       <b val="1"/>
-      <color rgb="FF3F3F3F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF3F3F76"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -162,14 +162,14 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <color rgb="FF9C6500"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FFFA7D00"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -183,187 +183,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -379,26 +379,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -427,11 +410,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -474,12 +463,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1">
@@ -503,128 +503,131 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="6" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1013,52 +1016,220 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.888888888888889" defaultRowHeight="14.4" outlineLevelRow="4"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.890909090909091" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="n">
+      <c r="A1" s="1" t="n">
         <v>12345</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>12348</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>123456</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>1234</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>90124</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>90124</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="1" t="n">
         <v>90124</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>12345678</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>12345678</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
login page front end test
</commit_message>
<xml_diff>
--- a/data/done.xlsx
+++ b/data/done.xlsx
@@ -1016,7 +1016,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A38"/>
+  <dimension ref="A1:A48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
@@ -1226,9 +1226,67 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="1" t="inlineStr">
         <is>
           <t>1234</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>123445</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>test123</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>12345678</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
autoconnect to server directly from main.py
</commit_message>
<xml_diff>
--- a/data/done.xlsx
+++ b/data/done.xlsx
@@ -1013,7 +1013,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A84"/>
+  <dimension ref="A1:A85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -1186,8 +1186,13 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="n">
+      <c r="A84" s="0" t="n">
         <v>90152</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>90124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>